<commit_message>
Scripting DPLKINV001-025 and DPLKINV001-026
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV001-025 -  Investasi - Reksadana Tambah, Ubah, View Detil & Hapus Data.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV001-025 -  Investasi - Reksadana Tambah, Ubah, View Detil & Hapus Data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8853E76A-21D4-4FD4-AF5D-C511755FEA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DPLKINV001" sheetId="2" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>SIDEBAR_MENU</t>
   </si>
@@ -46,36 +52,6 @@
     <t>PASSWORD</t>
   </si>
   <si>
-    <t>TEXT1</t>
-  </si>
-  <si>
-    <t>TEXT2</t>
-  </si>
-  <si>
-    <t>TEXT3</t>
-  </si>
-  <si>
-    <t>TEXT4</t>
-  </si>
-  <si>
-    <t>TEXT5</t>
-  </si>
-  <si>
-    <t>TEXT6</t>
-  </si>
-  <si>
-    <t>TEXT7</t>
-  </si>
-  <si>
-    <t>TEXT8</t>
-  </si>
-  <si>
-    <t>Putri</t>
-  </si>
-  <si>
-    <t>bni1234/</t>
-  </si>
-  <si>
     <t>MAIN_SIDEBAR</t>
   </si>
   <si>
@@ -97,44 +73,86 @@
     <t>Hapus Data Dapat dilakukan dengan baik</t>
   </si>
   <si>
-    <t>TEXT9</t>
-  </si>
-  <si>
-    <t>TEXT10</t>
-  </si>
-  <si>
-    <t>View :
-1. Klik icon Lihat Detail pada baris yang dituju</t>
-  </si>
-  <si>
-    <t>Tambah :
-1. Akses menu setup
-2. Klik tombol tambah
-3. Masukkan data
-4. Klik tombol Simpan</t>
-  </si>
-  <si>
-    <t>Ubah :
-1. Klik icon Ubah pada baris yang dituju
-2. Sesuaikan data yang ingin diubah
-3. Klik Simpan</t>
-  </si>
-  <si>
-    <t>Hapus :
-1. Klik icon Hapus pada baris yang dituju
-2. Klik tombol Ya, yakin!</t>
-  </si>
-  <si>
     <t>Normal - Investasi - Reksadana</t>
   </si>
   <si>
-    <t>INV001-025</t>
+    <t>DPLKINV001-025</t>
+  </si>
+  <si>
+    <t>Tambah Jenis Porto</t>
+  </si>
+  <si>
+    <t>View Jenis Porto</t>
+  </si>
+  <si>
+    <t>Ubah Jenis Porto</t>
+  </si>
+  <si>
+    <t>Hapus Jenis Porto</t>
+  </si>
+  <si>
+    <t>Reksadana</t>
+  </si>
+  <si>
+    <t>Jenis Porto</t>
+  </si>
+  <si>
+    <t>KODE_JENIS_PORTO</t>
+  </si>
+  <si>
+    <t>NAMA_JENIS_PORTO</t>
+  </si>
+  <si>
+    <t>STATUS_REGISTER</t>
+  </si>
+  <si>
+    <t>KETERANGAN_REGISTER</t>
+  </si>
+  <si>
+    <t>R91</t>
+  </si>
+  <si>
+    <t>Menunggu Register</t>
+  </si>
+  <si>
+    <t>Reksadana Campuran Syariah</t>
+  </si>
+  <si>
+    <t>PREPARATION</t>
+  </si>
+  <si>
+    <t>bni1234</t>
+  </si>
+  <si>
+    <t>Username : 32382;
+Password : bni1234;
+Kode Jenis Porto : R91</t>
+  </si>
+  <si>
+    <t>Username : 32382;
+Password : bni1234;
+Kode Jenis Porto : R91;
+Nama Jenis Porto : Reksadana Campuran Syariah</t>
+  </si>
+  <si>
+    <t>0 : Pending Register</t>
+  </si>
+  <si>
+    <t>Reksadana Pasar Uang Global</t>
+  </si>
+  <si>
+    <t>Username : 32382;
+Password : bni1234;
+Kode Jenis Porto : R91;
+Nama Jenis Porto : Reksadana Pasar Uang Global;
+Status Register : 0 : Pending Register;
+Keterangan Register : Menunggu Registrasi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -189,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -200,13 +218,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -520,274 +535,299 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
-    <col min="15" max="16" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="1"/>
-    <col min="21" max="21" width="12" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="1"/>
+    <col min="22" max="22" width="12" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="4">
+        <v>32382</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+    </row>
+    <row r="3" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="4" t="s">
+      <c r="E3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="4">
+        <v>32382</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="J3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="4" t="s">
+      <c r="L3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="4"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+    </row>
+    <row r="4" spans="1:22" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="4" t="s">
+      <c r="F4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="4">
+        <v>32382</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="4"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+    </row>
+    <row r="5" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>28</v>
-      </c>
+      <c r="F5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="4">
+        <v>32382</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
     </row>
-    <row r="2" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
-    <row r="3" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-    </row>
-    <row r="4" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-    </row>
-    <row r="5" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
-      <c r="F7" s="3"/>
       <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>